<commit_message>
Update model lastest versions of all sectors
</commit_message>
<xml_diff>
--- a/IPPU/A1_Inputs/NamesIPPU.xlsx
+++ b/IPPU/A1_Inputs/NamesIPPU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\Models_running\IPPU\A1_Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clgcr.sharepoint.com/sites/ClimateLeadGroup-NDC_Ecu/Documentos compartidos/ECU_NDC_model/setup_phase_4/IPPU_2025_01_14/A1_Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0088BB-B76D-4298-BB04-C870253F324E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CC0088BB-B76D-4298-BB04-C870253F324E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70F7BB3C-A45E-452E-BAC5-D9F22936649E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="75" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PrimaryTechologies" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="132">
   <si>
     <t>Code</t>
   </si>
@@ -761,7 +761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -815,9 +815,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1131,9 +1128,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8481359E-EA5D-427E-B167-F304C5744B8D}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,189 +1185,189 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="28" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="33" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="33" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="33" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="33" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="33" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="33" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="33" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1383,11 +1380,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD9285A-C0C4-429A-86A4-A14A7B7B5D2B}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,7 +1416,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="22" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>32</v>
       </c>
@@ -1427,17 +1424,6 @@
         <v>9</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="22" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="24" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1452,8 +1438,8 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7:C13"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1530,79 +1516,79 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="31" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="31" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="31" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="31" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="31" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1618,90 +1604,90 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="33" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="33" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="33" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="33" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="33" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="33" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="33" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="33" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1716,7 +1702,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67BB3B9D-BFA3-431B-ADD5-77A7C146800F}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1737,200 +1725,200 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="35" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="35" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="35" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="35" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="35" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="35" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="35" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="34" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="34" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="34" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="34" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="34" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="34" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="34" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1940,6 +1928,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8F814574E960A4499025803604D4DF4" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="314e7041d7d1561dbe33e80becf1c782">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4b2ff61d-e0c4-454b-ba72-44cf85c32a41" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="84c838da6aa04a0f137f8b0aba02cfe1" ns2:_="">
     <xsd:import namespace="4b2ff61d-e0c4-454b-ba72-44cf85c32a41"/>
@@ -2109,7 +2103,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2118,20 +2112,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61AC84A6-86D0-4D88-A04D-63963B151771}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AB75823-6ED7-48A7-B5B2-3D232D7B81BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{621F4BCF-90C0-45F1-AAD5-99E8997589EF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E48023-AEC6-40B0-B49D-05CE568A15B0}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AB75823-6ED7-48A7-B5B2-3D232D7B81BE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{621F4BCF-90C0-45F1-AAD5-99E8997589EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>